<commit_message>
Add hyvaksymiskirje-lahetetty for erillishaku
</commit_message>
<xml_diff>
--- a/src/test/resources/kkhaku_toisenasteen_valintatuloksella.xlsx
+++ b/src/test/resources/kkhaku_toisenasteen_valintatuloksella.xlsx
@@ -62,9 +62,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -163,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,6 +182,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,16 +214,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="9.15185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.15185185185185"/>
+    <col collapsed="false" hidden="false" max="258" min="1" style="1" width="9.83333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="259" style="0" width="9.83333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -250,150 +255,162 @@
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="5" t="n">
+        <v>42567</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>